<commit_message>
update to cleaning rules
</commit_message>
<xml_diff>
--- a/alerts/dictionary/cleaning_rules.xlsx
+++ b/alerts/dictionary/cleaning_rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Projects\deploying\git\report_factories_templates\alerts\dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89C8776-DA9B-4F41-97D5-B5D8A6793AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A62877-9BBA-4EAF-8EE6-DF70A15E0763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="explanations" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cleaning_rules - must be 1st sh'!$A$1:$C$701</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cleaning_rules - must be 1st sh'!$A$1:$C$702</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="780">
   <si>
     <t>bad_spelling</t>
   </si>
@@ -2366,6 +2366,9 @@
   </si>
   <si>
     <t>point_d_entree</t>
+  </si>
+  <si>
+    <t>vc</t>
   </si>
 </sst>
 </file>
@@ -2769,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK794"/>
+  <dimension ref="A1:AMK795"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C397" sqref="C397"/>
+    <sheetView tabSelected="1" topLeftCell="A405" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C417" sqref="C417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7361,7 +7364,7 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
-        <v>516</v>
+        <v>779</v>
       </c>
       <c r="B417" s="1" t="s">
         <v>503</v>
@@ -7372,7 +7375,7 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B418" s="1" t="s">
         <v>503</v>
@@ -7383,7 +7386,7 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>507</v>
+        <v>517</v>
       </c>
       <c r="B419" s="1" t="s">
         <v>503</v>
@@ -7394,10 +7397,10 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>292</v>
+        <v>503</v>
       </c>
       <c r="C420" s="1" t="s">
         <v>494</v>
@@ -7405,21 +7408,21 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>291</v>
+        <v>518</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>83</v>
+        <v>292</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>519</v>
+        <v>494</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>36</v>
+        <v>291</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>519</v>
@@ -7427,7 +7430,7 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>410</v>
+        <v>36</v>
       </c>
       <c r="B423" s="1" t="s">
         <v>37</v>
@@ -7438,7 +7441,7 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B424" s="1" t="s">
         <v>37</v>
@@ -7449,10 +7452,10 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>520</v>
+        <v>37</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>519</v>
@@ -7460,10 +7463,10 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>83</v>
+        <v>520</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>519</v>
@@ -7471,10 +7474,10 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>520</v>
+        <v>83</v>
       </c>
       <c r="C427" s="1" t="s">
         <v>519</v>
@@ -7482,7 +7485,7 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>521</v>
+        <v>409</v>
       </c>
       <c r="B428" s="1" t="s">
         <v>520</v>
@@ -7493,10 +7496,10 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
-        <v>394</v>
+        <v>521</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>83</v>
+        <v>520</v>
       </c>
       <c r="C429" s="1" t="s">
         <v>519</v>
@@ -7504,7 +7507,7 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>291</v>
+        <v>394</v>
       </c>
       <c r="B430" s="1" t="s">
         <v>83</v>
@@ -7515,10 +7518,10 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>408</v>
+        <v>291</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>520</v>
+        <v>83</v>
       </c>
       <c r="C431" s="1" t="s">
         <v>519</v>
@@ -7526,18 +7529,18 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="B432" s="9" t="s">
-        <v>523</v>
+        <v>408</v>
+      </c>
+      <c r="B432" s="1" t="s">
+        <v>520</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B433" s="9" t="s">
         <v>523</v>
@@ -7547,8 +7550,8 @@
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A434" s="7" t="s">
-        <v>526</v>
+      <c r="A434" s="1" t="s">
+        <v>525</v>
       </c>
       <c r="B434" s="9" t="s">
         <v>523</v>
@@ -7559,29 +7562,29 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B435" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A436" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="B435" s="1" t="s">
+      <c r="B436" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="C435" s="7" t="s">
+      <c r="C436" s="7" t="s">
         <v>524</v>
-      </c>
-    </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A436" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B436" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C436" s="1" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
-        <v>409</v>
+        <v>521</v>
       </c>
       <c r="B437" s="1" t="s">
         <v>408</v>
@@ -7592,18 +7595,18 @@
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A439" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C438" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A439" s="1">
-        <v>43308</v>
       </c>
       <c r="B439" s="1" t="s">
         <v>292</v>
@@ -7613,8 +7616,8 @@
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A440" s="1" t="s">
-        <v>530</v>
+      <c r="A440" s="1">
+        <v>43308</v>
       </c>
       <c r="B440" s="1" t="s">
         <v>292</v>
@@ -7625,7 +7628,7 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
-        <v>291</v>
+        <v>530</v>
       </c>
       <c r="B441" s="1" t="s">
         <v>292</v>
@@ -7636,43 +7639,43 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
-        <v>375</v>
+        <v>291</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>375</v>
+        <v>292</v>
       </c>
       <c r="C442" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C443" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C443" s="1" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
-        <v>291</v>
+        <v>374</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C444" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C444" s="3" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
-        <v>46</v>
+        <v>291</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>45</v>
+        <v>292</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>531</v>
@@ -7680,10 +7683,10 @@
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
-        <v>380</v>
+        <v>46</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C446" s="1" t="s">
         <v>531</v>
@@ -7691,10 +7694,10 @@
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>292</v>
+        <v>43</v>
       </c>
       <c r="C447" s="1" t="s">
         <v>531</v>
@@ -7702,29 +7705,29 @@
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A449" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="B448" s="1" t="s">
+      <c r="B449" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C448" s="1" t="s">
+      <c r="C449" s="1" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A449" s="1">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A450" s="1">
         <v>2</v>
-      </c>
-      <c r="B449" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C449" s="1" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A450" s="1" t="s">
-        <v>424</v>
       </c>
       <c r="B450" s="1" t="s">
         <v>422</v>
@@ -7734,19 +7737,19 @@
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A451" s="1">
-        <v>1</v>
+      <c r="A451" s="1" t="s">
+        <v>424</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C451" s="1" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A452" s="1" t="s">
-        <v>426</v>
+      <c r="A452" s="1">
+        <v>1</v>
       </c>
       <c r="B452" s="1" t="s">
         <v>425</v>
@@ -7757,7 +7760,7 @@
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B453" s="1" t="s">
         <v>425</v>
@@ -7768,7 +7771,7 @@
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B454" s="1" t="s">
         <v>425</v>
@@ -7779,10 +7782,10 @@
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
-        <v>291</v>
+        <v>428</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>83</v>
+        <v>425</v>
       </c>
       <c r="C455" s="1" t="s">
         <v>534</v>
@@ -7790,7 +7793,7 @@
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
-        <v>535</v>
+        <v>291</v>
       </c>
       <c r="B456" s="1" t="s">
         <v>83</v>
@@ -7801,7 +7804,7 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B457" s="1" t="s">
         <v>83</v>
@@ -7812,7 +7815,7 @@
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B458" s="1" t="s">
         <v>83</v>
@@ -7823,7 +7826,7 @@
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
-        <v>429</v>
+        <v>537</v>
       </c>
       <c r="B459" s="1" t="s">
         <v>83</v>
@@ -7834,10 +7837,10 @@
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>430</v>
+        <v>83</v>
       </c>
       <c r="C460" s="1" t="s">
         <v>534</v>
@@ -7845,10 +7848,10 @@
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
-        <v>538</v>
+        <v>394</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="C461" s="1" t="s">
         <v>534</v>
@@ -7856,10 +7859,10 @@
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C462" s="1" t="s">
         <v>534</v>
@@ -7867,10 +7870,10 @@
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
-        <v>427</v>
+        <v>539</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C463" s="1" t="s">
         <v>534</v>
@@ -7878,10 +7881,10 @@
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>534</v>
@@ -7889,18 +7892,18 @@
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" s="1" t="s">
-        <v>540</v>
+        <v>424</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>503</v>
+        <v>422</v>
       </c>
       <c r="C465" s="1" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
-        <v>507</v>
+        <v>540</v>
       </c>
       <c r="B466" s="1" t="s">
         <v>503</v>
@@ -7911,7 +7914,7 @@
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" s="1" t="s">
-        <v>542</v>
+        <v>507</v>
       </c>
       <c r="B467" s="1" t="s">
         <v>503</v>
@@ -7922,10 +7925,10 @@
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
-        <v>291</v>
+        <v>542</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>292</v>
+        <v>503</v>
       </c>
       <c r="C468" s="1" t="s">
         <v>541</v>
@@ -7933,7 +7936,7 @@
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" s="1" t="s">
-        <v>505</v>
+        <v>291</v>
       </c>
       <c r="B469" s="1" t="s">
         <v>292</v>
@@ -7944,10 +7947,10 @@
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" s="1" t="s">
-        <v>543</v>
+        <v>505</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>544</v>
+        <v>292</v>
       </c>
       <c r="C470" s="1" t="s">
         <v>541</v>
@@ -7955,7 +7958,7 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B471" s="1" t="s">
         <v>544</v>
@@ -7966,7 +7969,7 @@
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B472" s="1" t="s">
         <v>544</v>
@@ -7977,7 +7980,7 @@
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B473" s="1" t="s">
         <v>544</v>
@@ -7988,7 +7991,7 @@
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
-        <v>512</v>
+        <v>547</v>
       </c>
       <c r="B474" s="1" t="s">
         <v>544</v>
@@ -7999,10 +8002,10 @@
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" s="1" t="s">
-        <v>548</v>
+        <v>512</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>493</v>
+        <v>544</v>
       </c>
       <c r="C475" s="1" t="s">
         <v>541</v>
@@ -8010,7 +8013,7 @@
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" s="1" t="s">
-        <v>509</v>
+        <v>548</v>
       </c>
       <c r="B476" s="1" t="s">
         <v>493</v>
@@ -8021,7 +8024,7 @@
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" s="1" t="s">
-        <v>549</v>
+        <v>509</v>
       </c>
       <c r="B477" s="1" t="s">
         <v>493</v>
@@ -8032,7 +8035,7 @@
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B478" s="1" t="s">
         <v>493</v>
@@ -8043,10 +8046,10 @@
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" s="1" t="s">
-        <v>394</v>
+        <v>550</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>292</v>
+        <v>493</v>
       </c>
       <c r="C479" s="1" t="s">
         <v>541</v>
@@ -8054,18 +8057,18 @@
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" s="1" t="s">
-        <v>540</v>
+        <v>394</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C480" s="3" t="s">
-        <v>551</v>
+        <v>292</v>
+      </c>
+      <c r="C480" s="1" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B481" s="1" t="s">
         <v>503</v>
@@ -8076,10 +8079,10 @@
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" s="1" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="C482" s="3" t="s">
         <v>551</v>
@@ -8087,10 +8090,10 @@
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
       <c r="C483" s="3" t="s">
         <v>551</v>
@@ -8098,7 +8101,7 @@
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B484" s="1" t="s">
         <v>503</v>
@@ -8109,7 +8112,7 @@
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B485" s="1" t="s">
         <v>503</v>
@@ -8120,7 +8123,7 @@
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B486" s="1" t="s">
         <v>503</v>
@@ -8131,7 +8134,7 @@
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B487" s="1" t="s">
         <v>503</v>
@@ -8142,7 +8145,7 @@
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B488" s="1" t="s">
         <v>503</v>
@@ -8153,10 +8156,10 @@
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A489" s="1" t="s">
-        <v>291</v>
+        <v>558</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>292</v>
+        <v>503</v>
       </c>
       <c r="C489" s="3" t="s">
         <v>551</v>
@@ -8164,7 +8167,7 @@
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" s="1" t="s">
-        <v>505</v>
+        <v>291</v>
       </c>
       <c r="B490" s="1" t="s">
         <v>292</v>
@@ -8175,7 +8178,7 @@
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" s="1" t="s">
-        <v>383</v>
+        <v>505</v>
       </c>
       <c r="B491" s="1" t="s">
         <v>292</v>
@@ -8186,10 +8189,10 @@
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A492" s="1" t="s">
-        <v>559</v>
+        <v>383</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>510</v>
+        <v>292</v>
       </c>
       <c r="C492" s="3" t="s">
         <v>551</v>
@@ -8197,7 +8200,7 @@
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B493" s="1" t="s">
         <v>510</v>
@@ -8208,10 +8211,10 @@
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C494" s="3" t="s">
         <v>551</v>
@@ -8219,7 +8222,7 @@
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A495" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B495" s="1" t="s">
         <v>512</v>
@@ -8230,10 +8233,10 @@
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A496" s="1" t="s">
-        <v>487</v>
+        <v>562</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>493</v>
+        <v>512</v>
       </c>
       <c r="C496" s="3" t="s">
         <v>551</v>
@@ -8241,7 +8244,7 @@
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" s="1" t="s">
-        <v>563</v>
+        <v>487</v>
       </c>
       <c r="B497" s="1" t="s">
         <v>493</v>
@@ -8252,7 +8255,7 @@
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B498" s="1" t="s">
         <v>493</v>
@@ -8263,7 +8266,7 @@
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A499" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B499" s="1" t="s">
         <v>493</v>
@@ -8274,10 +8277,10 @@
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="C500" s="3" t="s">
         <v>551</v>
@@ -8285,10 +8288,10 @@
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A501" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
       <c r="C501" s="3" t="s">
         <v>551</v>
@@ -8296,21 +8299,21 @@
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502" s="1" t="s">
-        <v>542</v>
+        <v>567</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="C502" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C502" s="3" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503" s="1" t="s">
-        <v>509</v>
+        <v>542</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>493</v>
+        <v>503</v>
       </c>
       <c r="C503" s="1" t="s">
         <v>551</v>
@@ -8318,29 +8321,29 @@
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A504" s="1" t="s">
-        <v>568</v>
+        <v>509</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
       <c r="C504" s="1" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A505" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B505" s="6" t="s">
-        <v>7</v>
+      <c r="A505" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>512</v>
       </c>
       <c r="C505" s="1" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A506" s="6" t="s">
-        <v>570</v>
+        <v>7</v>
       </c>
       <c r="B506" s="6" t="s">
         <v>7</v>
@@ -8351,7 +8354,7 @@
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A507" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B507" s="6" t="s">
         <v>7</v>
@@ -8362,7 +8365,7 @@
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A508" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B508" s="6" t="s">
         <v>7</v>
@@ -8373,18 +8376,18 @@
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A509" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B509" s="6" t="s">
-        <v>573</v>
+        <v>7</v>
       </c>
       <c r="C509" s="1" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A510" s="1" t="s">
-        <v>574</v>
+      <c r="A510" s="6" t="s">
+        <v>573</v>
       </c>
       <c r="B510" s="6" t="s">
         <v>573</v>
@@ -8395,7 +8398,7 @@
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A511" s="1" t="s">
-        <v>348</v>
+        <v>574</v>
       </c>
       <c r="B511" s="6" t="s">
         <v>573</v>
@@ -8406,7 +8409,7 @@
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A512" s="1" t="s">
-        <v>575</v>
+        <v>348</v>
       </c>
       <c r="B512" s="6" t="s">
         <v>573</v>
@@ -8416,11 +8419,11 @@
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A513" s="6" t="s">
-        <v>4</v>
+      <c r="A513" s="1" t="s">
+        <v>575</v>
       </c>
       <c r="B513" s="6" t="s">
-        <v>15</v>
+        <v>573</v>
       </c>
       <c r="C513" s="1" t="s">
         <v>569</v>
@@ -8428,7 +8431,7 @@
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A514" s="6" t="s">
-        <v>576</v>
+        <v>4</v>
       </c>
       <c r="B514" s="6" t="s">
         <v>15</v>
@@ -8439,7 +8442,7 @@
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A515" s="6" t="s">
-        <v>15</v>
+        <v>576</v>
       </c>
       <c r="B515" s="6" t="s">
         <v>15</v>
@@ -8450,7 +8453,7 @@
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A516" s="6" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="B516" s="6" t="s">
         <v>15</v>
@@ -8461,7 +8464,7 @@
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A517" s="6" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="B517" s="6" t="s">
         <v>15</v>
@@ -8472,7 +8475,7 @@
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A518" s="6" t="s">
-        <v>577</v>
+        <v>21</v>
       </c>
       <c r="B518" s="6" t="s">
         <v>15</v>
@@ -8483,7 +8486,7 @@
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A519" s="6" t="s">
-        <v>366</v>
+        <v>577</v>
       </c>
       <c r="B519" s="6" t="s">
         <v>15</v>
@@ -8494,7 +8497,7 @@
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A520" s="6" t="s">
-        <v>578</v>
+        <v>366</v>
       </c>
       <c r="B520" s="6" t="s">
         <v>15</v>
@@ -8505,7 +8508,7 @@
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A521" s="6" t="s">
-        <v>48</v>
+        <v>578</v>
       </c>
       <c r="B521" s="6" t="s">
         <v>15</v>
@@ -8516,7 +8519,7 @@
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A522" s="6" t="s">
-        <v>579</v>
+        <v>48</v>
       </c>
       <c r="B522" s="6" t="s">
         <v>15</v>
@@ -8527,7 +8530,7 @@
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A523" s="6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B523" s="6" t="s">
         <v>15</v>
@@ -8538,7 +8541,7 @@
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A524" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B524" s="6" t="s">
         <v>15</v>
@@ -8548,11 +8551,11 @@
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A525" s="1" t="s">
-        <v>582</v>
+      <c r="A525" s="6" t="s">
+        <v>581</v>
       </c>
       <c r="B525" s="6" t="s">
-        <v>583</v>
+        <v>15</v>
       </c>
       <c r="C525" s="1" t="s">
         <v>569</v>
@@ -8560,7 +8563,7 @@
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A526" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B526" s="6" t="s">
         <v>583</v>
@@ -8571,7 +8574,7 @@
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A527" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B527" s="6" t="s">
         <v>583</v>
@@ -8581,8 +8584,8 @@
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A528" s="6" t="s">
-        <v>583</v>
+      <c r="A528" s="1" t="s">
+        <v>585</v>
       </c>
       <c r="B528" s="6" t="s">
         <v>583</v>
@@ -8592,8 +8595,8 @@
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A529" s="1" t="s">
-        <v>586</v>
+      <c r="A529" s="6" t="s">
+        <v>583</v>
       </c>
       <c r="B529" s="6" t="s">
         <v>583</v>
@@ -8603,8 +8606,8 @@
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A530" s="6" t="s">
-        <v>19</v>
+      <c r="A530" s="1" t="s">
+        <v>586</v>
       </c>
       <c r="B530" s="6" t="s">
         <v>583</v>
@@ -8614,8 +8617,8 @@
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A531" s="1" t="s">
-        <v>587</v>
+      <c r="A531" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="B531" s="6" t="s">
         <v>583</v>
@@ -8626,7 +8629,7 @@
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A532" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B532" s="6" t="s">
         <v>583</v>
@@ -8637,7 +8640,7 @@
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A533" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B533" s="6" t="s">
         <v>583</v>
@@ -8648,7 +8651,7 @@
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A534" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B534" s="6" t="s">
         <v>583</v>
@@ -8659,7 +8662,7 @@
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A535" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B535" s="6" t="s">
         <v>583</v>
@@ -8670,7 +8673,7 @@
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A536" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B536" s="6" t="s">
         <v>583</v>
@@ -8680,8 +8683,8 @@
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A537" s="6" t="s">
-        <v>593</v>
+      <c r="A537" s="1" t="s">
+        <v>592</v>
       </c>
       <c r="B537" s="6" t="s">
         <v>583</v>
@@ -8691,8 +8694,8 @@
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A538" s="1" t="s">
-        <v>594</v>
+      <c r="A538" s="6" t="s">
+        <v>593</v>
       </c>
       <c r="B538" s="6" t="s">
         <v>583</v>
@@ -8703,7 +8706,7 @@
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A539" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B539" s="6" t="s">
         <v>583</v>
@@ -8714,7 +8717,7 @@
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A540" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B540" s="6" t="s">
         <v>583</v>
@@ -8725,7 +8728,7 @@
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A541" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B541" s="6" t="s">
         <v>583</v>
@@ -8735,11 +8738,11 @@
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A542" s="6" t="s">
-        <v>24</v>
+      <c r="A542" s="1" t="s">
+        <v>597</v>
       </c>
       <c r="B542" s="6" t="s">
-        <v>24</v>
+        <v>583</v>
       </c>
       <c r="C542" s="1" t="s">
         <v>569</v>
@@ -8747,7 +8750,7 @@
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A543" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B543" s="6" t="s">
         <v>24</v>
@@ -8758,10 +8761,10 @@
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A544" s="6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B544" s="6" t="s">
-        <v>253</v>
+        <v>24</v>
       </c>
       <c r="C544" s="1" t="s">
         <v>569</v>
@@ -8769,7 +8772,7 @@
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A545" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B545" s="6" t="s">
         <v>253</v>
@@ -8780,10 +8783,10 @@
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A546" s="6" t="s">
-        <v>598</v>
+        <v>28</v>
       </c>
       <c r="B546" s="6" t="s">
-        <v>598</v>
+        <v>253</v>
       </c>
       <c r="C546" s="1" t="s">
         <v>569</v>
@@ -8791,7 +8794,7 @@
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A547" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B547" s="6" t="s">
         <v>598</v>
@@ -8802,10 +8805,10 @@
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A548" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B548" s="6" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C548" s="1" t="s">
         <v>569</v>
@@ -8813,21 +8816,21 @@
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A549" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B549" s="6" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C549" s="1" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A550" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B550" s="1" t="s">
-        <v>603</v>
+      <c r="A550" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="B550" s="6" t="s">
+        <v>602</v>
       </c>
       <c r="C550" s="1" t="s">
         <v>569</v>
@@ -8835,29 +8838,29 @@
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A551" s="1" t="s">
-        <v>379</v>
+        <v>291</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>378</v>
+        <v>603</v>
       </c>
       <c r="C551" s="1" t="s">
-        <v>604</v>
+        <v>569</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A552" s="1" t="s">
-        <v>605</v>
+        <v>379</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>45</v>
+        <v>378</v>
       </c>
       <c r="C552" s="1" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A553" s="9" t="s">
-        <v>46</v>
+      <c r="A553" s="1" t="s">
+        <v>605</v>
       </c>
       <c r="B553" s="1" t="s">
         <v>45</v>
@@ -8867,11 +8870,11 @@
       </c>
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A554" s="1" t="s">
-        <v>43</v>
+      <c r="A554" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C554" s="1" t="s">
         <v>604</v>
@@ -8879,10 +8882,10 @@
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A555" s="1" t="s">
-        <v>606</v>
+        <v>43</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>390</v>
+        <v>43</v>
       </c>
       <c r="C555" s="1" t="s">
         <v>604</v>
@@ -8890,10 +8893,10 @@
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A556" s="1" t="s">
-        <v>291</v>
+        <v>606</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>292</v>
+        <v>390</v>
       </c>
       <c r="C556" s="1" t="s">
         <v>604</v>
@@ -8907,37 +8910,37 @@
         <v>292</v>
       </c>
       <c r="C557" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A558" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C558" s="1" t="s">
         <v>607</v>
-      </c>
-    </row>
-    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A558" s="1">
-        <v>2</v>
-      </c>
-      <c r="B558" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C558" s="1" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A559" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>37</v>
+        <v>408</v>
       </c>
       <c r="C559" s="1" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A560" s="1" t="s">
-        <v>291</v>
+      <c r="A560" s="1">
+        <v>1</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="C560" s="1" t="s">
         <v>608</v>
@@ -8945,7 +8948,7 @@
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A561" s="1" t="s">
-        <v>394</v>
+        <v>291</v>
       </c>
       <c r="B561" s="1" t="s">
         <v>83</v>
@@ -8956,65 +8959,65 @@
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A562" s="1" t="s">
-        <v>438</v>
+        <v>394</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>292</v>
+        <v>83</v>
       </c>
       <c r="C562" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A563" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C563" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A564" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B563" s="1" t="s">
+      <c r="B564" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="C563" s="1" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A564" s="1">
-        <v>0</v>
-      </c>
-      <c r="B564" s="1" t="s">
-        <v>405</v>
       </c>
       <c r="C564" s="1" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A565" s="1" t="s">
+      <c r="A565" s="1">
+        <v>0</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C565" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A566" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="B565" s="1" t="s">
+      <c r="B566" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="C565" s="1" t="s">
+      <c r="C566" s="1" t="s">
         <v>614</v>
-      </c>
-    </row>
-    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A566" s="1">
-        <v>1</v>
-      </c>
-      <c r="B566" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="C566" s="1" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A567" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C567" s="1" t="s">
         <v>615</v>
@@ -9022,18 +9025,18 @@
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A568" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>83</v>
+        <v>400</v>
       </c>
       <c r="C568" s="1" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A569" s="1" t="s">
-        <v>291</v>
+      <c r="A569" s="1">
+        <v>3</v>
       </c>
       <c r="B569" s="1" t="s">
         <v>83</v>
@@ -9043,8 +9046,8 @@
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A570" s="1">
-        <v>43440</v>
+      <c r="A570" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="B570" s="1" t="s">
         <v>83</v>
@@ -9054,22 +9057,22 @@
       </c>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A571" s="1" t="s">
-        <v>616</v>
+      <c r="A571" s="1">
+        <v>43440</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>617</v>
+        <v>83</v>
       </c>
       <c r="C571" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A572" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>512</v>
+        <v>617</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>618</v>
@@ -9077,10 +9080,10 @@
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A573" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>621</v>
+        <v>512</v>
       </c>
       <c r="C573" s="1" t="s">
         <v>618</v>
@@ -9088,7 +9091,7 @@
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A574" s="1" t="s">
-        <v>501</v>
+        <v>620</v>
       </c>
       <c r="B574" s="1" t="s">
         <v>621</v>
@@ -9099,7 +9102,7 @@
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A575" s="1" t="s">
-        <v>622</v>
+        <v>501</v>
       </c>
       <c r="B575" s="1" t="s">
         <v>621</v>
@@ -9110,7 +9113,7 @@
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A576" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B576" s="1" t="s">
         <v>621</v>
@@ -9121,10 +9124,10 @@
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A577" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>509</v>
+        <v>621</v>
       </c>
       <c r="C577" s="1" t="s">
         <v>618</v>
@@ -9132,7 +9135,7 @@
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A578" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B578" s="1" t="s">
         <v>509</v>
@@ -9143,7 +9146,7 @@
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A579" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B579" s="1" t="s">
         <v>509</v>
@@ -9154,7 +9157,7 @@
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A580" s="1" t="s">
-        <v>413</v>
+        <v>626</v>
       </c>
       <c r="B580" s="1" t="s">
         <v>509</v>
@@ -9165,10 +9168,10 @@
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A581" s="1" t="s">
-        <v>627</v>
+        <v>413</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C581" s="1" t="s">
         <v>618</v>
@@ -9176,10 +9179,10 @@
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A582" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>621</v>
+        <v>507</v>
       </c>
       <c r="C582" s="1" t="s">
         <v>618</v>
@@ -9187,10 +9190,10 @@
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A583" s="1" t="s">
-        <v>517</v>
+        <v>628</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>507</v>
+        <v>621</v>
       </c>
       <c r="C583" s="1" t="s">
         <v>618</v>
@@ -9198,7 +9201,7 @@
     </row>
     <row r="584" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A584" s="1" t="s">
-        <v>629</v>
+        <v>517</v>
       </c>
       <c r="B584" s="1" t="s">
         <v>507</v>
@@ -9209,7 +9212,7 @@
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A585" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B585" s="1" t="s">
         <v>507</v>
@@ -9220,18 +9223,18 @@
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A586" s="1" t="s">
-        <v>505</v>
+        <v>630</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>292</v>
+        <v>507</v>
       </c>
       <c r="C586" s="1" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="587" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A587" s="9" t="s">
-        <v>291</v>
+      <c r="A587" s="1" t="s">
+        <v>505</v>
       </c>
       <c r="B587" s="1" t="s">
         <v>292</v>
@@ -9247,13 +9250,13 @@
       <c r="B588" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C588" s="7" t="s">
-        <v>631</v>
+      <c r="C588" s="1" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="589" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A589" s="9" t="s">
-        <v>438</v>
+        <v>291</v>
       </c>
       <c r="B589" s="1" t="s">
         <v>292</v>
@@ -9263,33 +9266,33 @@
       </c>
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A590" s="1" t="s">
-        <v>291</v>
+      <c r="A590" s="9" t="s">
+        <v>438</v>
       </c>
       <c r="B590" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C590" s="1" t="s">
-        <v>632</v>
+      <c r="C590" s="7" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="591" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A591" s="1" t="s">
-        <v>396</v>
+        <v>291</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>397</v>
+        <v>292</v>
       </c>
       <c r="C591" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="592" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A592" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C592" s="1" t="s">
         <v>633</v>
@@ -9297,10 +9300,10 @@
     </row>
     <row r="593" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A593" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>83</v>
+        <v>400</v>
       </c>
       <c r="C593" s="1" t="s">
         <v>633</v>
@@ -9308,7 +9311,7 @@
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A594" s="1" t="s">
-        <v>291</v>
+        <v>401</v>
       </c>
       <c r="B594" s="1" t="s">
         <v>83</v>
@@ -9322,7 +9325,7 @@
         <v>291</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>634</v>
+        <v>83</v>
       </c>
       <c r="C595" s="1" t="s">
         <v>633</v>
@@ -9330,18 +9333,18 @@
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A596" s="1" t="s">
-        <v>635</v>
+        <v>291</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>397</v>
+        <v>634</v>
       </c>
       <c r="C596" s="1" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A597" s="7" t="s">
-        <v>636</v>
+      <c r="A597" s="1" t="s">
+        <v>635</v>
       </c>
       <c r="B597" s="1" t="s">
         <v>397</v>
@@ -9352,7 +9355,7 @@
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A598" s="7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B598" s="1" t="s">
         <v>397</v>
@@ -9363,7 +9366,7 @@
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A599" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B599" s="1" t="s">
         <v>397</v>
@@ -9374,7 +9377,7 @@
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A600" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B600" s="1" t="s">
         <v>397</v>
@@ -9385,7 +9388,7 @@
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A601" s="7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B601" s="1" t="s">
         <v>397</v>
@@ -9396,7 +9399,7 @@
     </row>
     <row r="602" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A602" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B602" s="1" t="s">
         <v>397</v>
@@ -9407,7 +9410,7 @@
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A603" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B603" s="1" t="s">
         <v>397</v>
@@ -9417,19 +9420,19 @@
       </c>
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A604" s="9" t="s">
-        <v>371</v>
+      <c r="A604" s="7" t="s">
+        <v>642</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C604" s="9" t="s">
-        <v>643</v>
+        <v>397</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="605" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A605" s="9" t="s">
-        <v>292</v>
+        <v>371</v>
       </c>
       <c r="B605" s="1" t="s">
         <v>83</v>
@@ -9440,10 +9443,10 @@
     </row>
     <row r="606" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A606" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="B606" s="9" t="s">
-        <v>645</v>
+        <v>292</v>
+      </c>
+      <c r="B606" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C606" s="9" t="s">
         <v>643</v>
@@ -9451,7 +9454,7 @@
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A607" s="9" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B607" s="9" t="s">
         <v>645</v>
@@ -9462,7 +9465,7 @@
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A608" s="9" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B608" s="9" t="s">
         <v>645</v>
@@ -9473,7 +9476,7 @@
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A609" s="9" t="s">
-        <v>383</v>
+        <v>647</v>
       </c>
       <c r="B609" s="9" t="s">
         <v>645</v>
@@ -9484,10 +9487,10 @@
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A610" s="9" t="s">
-        <v>648</v>
-      </c>
-      <c r="B610" s="1" t="s">
-        <v>83</v>
+        <v>383</v>
+      </c>
+      <c r="B610" s="9" t="s">
+        <v>645</v>
       </c>
       <c r="C610" s="9" t="s">
         <v>643</v>
@@ -9495,10 +9498,10 @@
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A611" s="9" t="s">
-        <v>649</v>
-      </c>
-      <c r="B611" s="9" t="s">
-        <v>645</v>
+        <v>648</v>
+      </c>
+      <c r="B611" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C611" s="9" t="s">
         <v>643</v>
@@ -9506,7 +9509,7 @@
     </row>
     <row r="612" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A612" s="9" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B612" s="9" t="s">
         <v>645</v>
@@ -9517,7 +9520,7 @@
     </row>
     <row r="613" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A613" s="9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B613" s="9" t="s">
         <v>645</v>
@@ -9528,7 +9531,7 @@
     </row>
     <row r="614" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A614" s="9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B614" s="9" t="s">
         <v>645</v>
@@ -9538,22 +9541,22 @@
       </c>
     </row>
     <row r="615" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A615" s="9">
-        <v>1</v>
-      </c>
-      <c r="B615" s="1" t="s">
-        <v>83</v>
+      <c r="A615" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="B615" s="9" t="s">
+        <v>645</v>
       </c>
       <c r="C615" s="9" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="616" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A616" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="B616" s="9" t="s">
-        <v>654</v>
+      <c r="A616" s="9">
+        <v>1</v>
+      </c>
+      <c r="B616" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C616" s="9" t="s">
         <v>643</v>
@@ -9561,7 +9564,7 @@
     </row>
     <row r="617" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A617" s="9" t="s">
-        <v>391</v>
+        <v>653</v>
       </c>
       <c r="B617" s="9" t="s">
         <v>654</v>
@@ -9572,7 +9575,7 @@
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A618" s="9" t="s">
-        <v>655</v>
+        <v>391</v>
       </c>
       <c r="B618" s="9" t="s">
         <v>654</v>
@@ -9583,7 +9586,7 @@
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A619" s="9" t="s">
-        <v>633</v>
+        <v>655</v>
       </c>
       <c r="B619" s="9" t="s">
         <v>654</v>
@@ -9594,7 +9597,7 @@
     </row>
     <row r="620" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A620" s="9" t="s">
-        <v>656</v>
+        <v>633</v>
       </c>
       <c r="B620" s="9" t="s">
         <v>654</v>
@@ -9605,7 +9608,7 @@
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A621" s="9" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B621" s="9" t="s">
         <v>654</v>
@@ -9616,7 +9619,7 @@
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A622" s="9" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B622" s="9" t="s">
         <v>654</v>
@@ -9627,7 +9630,7 @@
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A623" s="9" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B623" s="9" t="s">
         <v>654</v>
@@ -9638,10 +9641,10 @@
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A624" s="9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B624" s="9" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="C624" s="9" t="s">
         <v>643</v>
@@ -9649,7 +9652,7 @@
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A625" s="9" t="s">
-        <v>652</v>
+        <v>659</v>
       </c>
       <c r="B625" s="9" t="s">
         <v>645</v>
@@ -9660,7 +9663,7 @@
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A626" s="9" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="B626" s="9" t="s">
         <v>645</v>
@@ -9670,8 +9673,8 @@
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A627" s="4" t="s">
-        <v>661</v>
+      <c r="A627" s="9" t="s">
+        <v>660</v>
       </c>
       <c r="B627" s="9" t="s">
         <v>645</v>
@@ -9681,8 +9684,8 @@
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A628" s="9" t="s">
-        <v>662</v>
+      <c r="A628" s="4" t="s">
+        <v>661</v>
       </c>
       <c r="B628" s="9" t="s">
         <v>645</v>
@@ -9692,19 +9695,19 @@
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A629" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="B629" s="1" t="s">
+      <c r="A629" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="B629" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="C629" s="1" t="s">
+      <c r="C629" s="9" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A630" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B630" s="1" t="s">
         <v>645</v>
@@ -9715,10 +9718,10 @@
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A631" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>83</v>
+        <v>645</v>
       </c>
       <c r="C631" s="1" t="s">
         <v>643</v>
@@ -9726,10 +9729,10 @@
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A632" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>645</v>
+        <v>83</v>
       </c>
       <c r="C632" s="1" t="s">
         <v>643</v>
@@ -9737,7 +9740,7 @@
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A633" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B633" s="1" t="s">
         <v>645</v>
@@ -9748,10 +9751,10 @@
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A634" s="1" t="s">
-        <v>394</v>
+        <v>667</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>395</v>
+        <v>645</v>
       </c>
       <c r="C634" s="1" t="s">
         <v>643</v>
@@ -9759,10 +9762,10 @@
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A635" s="1" t="s">
-        <v>668</v>
+        <v>394</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>83</v>
+        <v>395</v>
       </c>
       <c r="C635" s="1" t="s">
         <v>643</v>
@@ -9770,7 +9773,7 @@
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A636" s="1" t="s">
-        <v>291</v>
+        <v>668</v>
       </c>
       <c r="B636" s="1" t="s">
         <v>83</v>
@@ -9784,10 +9787,10 @@
         <v>291</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>292</v>
+        <v>83</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>657</v>
+        <v>643</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.25">
@@ -9798,15 +9801,15 @@
         <v>292</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>669</v>
+        <v>657</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A639" s="1" t="s">
-        <v>46</v>
+        <v>291</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>45</v>
+        <v>292</v>
       </c>
       <c r="C639" s="1" t="s">
         <v>669</v>
@@ -9814,7 +9817,7 @@
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A640" s="1" t="s">
-        <v>389</v>
+        <v>46</v>
       </c>
       <c r="B640" s="1" t="s">
         <v>45</v>
@@ -9825,7 +9828,7 @@
     </row>
     <row r="641" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A641" s="1" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B641" s="1" t="s">
         <v>45</v>
@@ -9836,10 +9839,10 @@
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A642" s="1" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C642" s="1" t="s">
         <v>669</v>
@@ -9847,7 +9850,7 @@
     </row>
     <row r="643" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A643" s="1" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="B643" s="1" t="s">
         <v>43</v>
@@ -9858,21 +9861,21 @@
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A644" s="1" t="s">
-        <v>670</v>
+        <v>380</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>598</v>
+        <v>43</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A645" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B645" s="1" t="s">
-        <v>570</v>
+        <v>598</v>
       </c>
       <c r="C645" s="1" t="s">
         <v>671</v>
@@ -9880,10 +9883,10 @@
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A646" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>593</v>
+        <v>570</v>
       </c>
       <c r="C646" s="1" t="s">
         <v>671</v>
@@ -9891,10 +9894,10 @@
     </row>
     <row r="647" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A647" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="C647" s="1" t="s">
         <v>671</v>
@@ -9902,10 +9905,10 @@
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A648" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="C648" s="1" t="s">
         <v>671</v>
@@ -9913,10 +9916,10 @@
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A649" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="B649" s="6" t="s">
-        <v>4</v>
+        <v>675</v>
+      </c>
+      <c r="B649" s="1" t="s">
+        <v>597</v>
       </c>
       <c r="C649" s="1" t="s">
         <v>671</v>
@@ -9924,10 +9927,10 @@
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A650" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="B650" s="1" t="s">
-        <v>7</v>
+        <v>676</v>
+      </c>
+      <c r="B650" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="C650" s="1" t="s">
         <v>671</v>
@@ -9935,10 +9938,10 @@
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A651" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C651" s="1" t="s">
         <v>671</v>
@@ -9946,18 +9949,18 @@
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A652" s="1" t="s">
-        <v>291</v>
+        <v>678</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>292</v>
+        <v>15</v>
       </c>
       <c r="C652" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A653" s="3" t="s">
-        <v>679</v>
+      <c r="A653" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="B653" s="1" t="s">
         <v>292</v>
@@ -9968,7 +9971,7 @@
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A654" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B654" s="1" t="s">
         <v>292</v>
@@ -9978,11 +9981,11 @@
       </c>
     </row>
     <row r="655" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A655" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="B655" s="6" t="s">
-        <v>104</v>
+      <c r="A655" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="B655" s="1" t="s">
+        <v>292</v>
       </c>
       <c r="C655" s="1" t="s">
         <v>671</v>
@@ -9990,7 +9993,7 @@
     </row>
     <row r="656" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A656" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B656" s="6" t="s">
         <v>104</v>
@@ -10001,7 +10004,7 @@
     </row>
     <row r="657" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A657" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B657" s="6" t="s">
         <v>104</v>
@@ -10011,22 +10014,22 @@
       </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A658" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="B658" s="1" t="s">
-        <v>21</v>
+      <c r="A658" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B658" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="C658" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="659" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A659" s="1" t="s">
-        <v>685</v>
+      <c r="A659" s="3" t="s">
+        <v>684</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>577</v>
+        <v>21</v>
       </c>
       <c r="C659" s="1" t="s">
         <v>671</v>
@@ -10034,21 +10037,21 @@
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A660" s="1" t="s">
-        <v>232</v>
+        <v>685</v>
       </c>
       <c r="B660" s="1" t="s">
-        <v>24</v>
+        <v>577</v>
       </c>
       <c r="C660" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A661" s="3" t="s">
-        <v>686</v>
+      <c r="A661" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C661" s="1" t="s">
         <v>671</v>
@@ -10056,10 +10059,10 @@
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A662" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B662" s="3" t="s">
-        <v>189</v>
+        <v>686</v>
+      </c>
+      <c r="B662" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C662" s="1" t="s">
         <v>671</v>
@@ -10067,10 +10070,10 @@
     </row>
     <row r="663" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A663" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="B663" s="1" t="s">
-        <v>26</v>
+        <v>188</v>
+      </c>
+      <c r="B663" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="C663" s="1" t="s">
         <v>671</v>
@@ -10078,7 +10081,7 @@
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A664" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B664" s="1" t="s">
         <v>26</v>
@@ -10088,8 +10091,8 @@
       </c>
     </row>
     <row r="665" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A665" s="1" t="s">
-        <v>26</v>
+      <c r="A665" s="3" t="s">
+        <v>688</v>
       </c>
       <c r="B665" s="1" t="s">
         <v>26</v>
@@ -10100,7 +10103,7 @@
     </row>
     <row r="666" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A666" s="1" t="s">
-        <v>689</v>
+        <v>26</v>
       </c>
       <c r="B666" s="1" t="s">
         <v>26</v>
@@ -10110,8 +10113,8 @@
       </c>
     </row>
     <row r="667" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A667" s="3" t="s">
-        <v>690</v>
+      <c r="A667" s="1" t="s">
+        <v>689</v>
       </c>
       <c r="B667" s="1" t="s">
         <v>26</v>
@@ -10122,7 +10125,7 @@
     </row>
     <row r="668" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A668" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B668" s="1" t="s">
         <v>26</v>
@@ -10133,7 +10136,7 @@
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A669" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B669" s="1" t="s">
         <v>26</v>
@@ -10144,20 +10147,20 @@
     </row>
     <row r="670" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A670" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="B670" s="3" t="s">
-        <v>28</v>
+        <v>692</v>
+      </c>
+      <c r="B670" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C670" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="671" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A671" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="B671" s="1" t="s">
+      <c r="A671" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="B671" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C671" s="1" t="s">
@@ -10165,10 +10168,10 @@
       </c>
     </row>
     <row r="672" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A672" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B672" s="3" t="s">
+      <c r="A672" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B672" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C672" s="1" t="s">
@@ -10177,7 +10180,7 @@
     </row>
     <row r="673" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A673" s="3" t="s">
-        <v>695</v>
+        <v>28</v>
       </c>
       <c r="B673" s="3" t="s">
         <v>28</v>
@@ -10188,9 +10191,9 @@
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A674" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="B674" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="B674" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C674" s="1" t="s">
@@ -10198,8 +10201,8 @@
       </c>
     </row>
     <row r="675" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A675" s="1" t="s">
-        <v>697</v>
+      <c r="A675" s="3" t="s">
+        <v>696</v>
       </c>
       <c r="B675" s="1" t="s">
         <v>28</v>
@@ -10210,7 +10213,7 @@
     </row>
     <row r="676" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A676" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B676" s="1" t="s">
         <v>28</v>
@@ -10221,10 +10224,10 @@
     </row>
     <row r="677" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A677" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="B677" s="6" t="s">
-        <v>48</v>
+        <v>695</v>
+      </c>
+      <c r="B677" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C677" s="1" t="s">
         <v>671</v>
@@ -10232,7 +10235,7 @@
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A678" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B678" s="6" t="s">
         <v>48</v>
@@ -10243,7 +10246,7 @@
     </row>
     <row r="679" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A679" s="1" t="s">
-        <v>47</v>
+        <v>699</v>
       </c>
       <c r="B679" s="6" t="s">
         <v>48</v>
@@ -10253,11 +10256,11 @@
       </c>
     </row>
     <row r="680" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A680" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="B680" s="1" t="s">
-        <v>580</v>
+      <c r="A680" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B680" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C680" s="1" t="s">
         <v>671</v>
@@ -10265,7 +10268,7 @@
     </row>
     <row r="681" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A681" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B681" s="1" t="s">
         <v>580</v>
@@ -10276,7 +10279,7 @@
     </row>
     <row r="682" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A682" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B682" s="1" t="s">
         <v>580</v>
@@ -10287,7 +10290,7 @@
     </row>
     <row r="683" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A683" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B683" s="1" t="s">
         <v>580</v>
@@ -10298,7 +10301,7 @@
     </row>
     <row r="684" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A684" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B684" s="1" t="s">
         <v>580</v>
@@ -10309,32 +10312,32 @@
     </row>
     <row r="685" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A685" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>35</v>
+        <v>580</v>
       </c>
       <c r="C685" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="686" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A686" s="1" t="s">
-        <v>706</v>
+      <c r="A686" s="3" t="s">
+        <v>705</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>595</v>
+        <v>35</v>
       </c>
       <c r="C686" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="687" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A687" s="3" t="s">
-        <v>707</v>
+      <c r="A687" s="1" t="s">
+        <v>706</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>581</v>
+        <v>595</v>
       </c>
       <c r="C687" s="1" t="s">
         <v>671</v>
@@ -10342,10 +10345,10 @@
     </row>
     <row r="688" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A688" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
       <c r="C688" s="1" t="s">
         <v>671</v>
@@ -10353,10 +10356,10 @@
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A689" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>26</v>
+        <v>571</v>
       </c>
       <c r="C689" s="1" t="s">
         <v>671</v>
@@ -10364,7 +10367,7 @@
     </row>
     <row r="690" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A690" s="3" t="s">
-        <v>253</v>
+        <v>709</v>
       </c>
       <c r="B690" s="1" t="s">
         <v>26</v>
@@ -10375,10 +10378,10 @@
     </row>
     <row r="691" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A691" s="3" t="s">
-        <v>438</v>
+        <v>253</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>292</v>
+        <v>26</v>
       </c>
       <c r="C691" s="1" t="s">
         <v>671</v>
@@ -10386,7 +10389,7 @@
     </row>
     <row r="692" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A692" s="3" t="s">
-        <v>291</v>
+        <v>438</v>
       </c>
       <c r="B692" s="1" t="s">
         <v>292</v>
@@ -10396,33 +10399,33 @@
       </c>
     </row>
     <row r="693" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A693" s="7" t="s">
+      <c r="A693" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B693" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C693" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A694" s="7" t="s">
         <v>710</v>
       </c>
-      <c r="B693" s="1" t="s">
+      <c r="B694" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C693" s="7" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="694" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A694" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="B694" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="C694" s="1" t="s">
+      <c r="C694" s="7" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="695" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A695" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>26</v>
+        <v>598</v>
       </c>
       <c r="C695" s="1" t="s">
         <v>671</v>
@@ -10430,18 +10433,18 @@
     </row>
     <row r="696" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A696" s="1" t="s">
-        <v>505</v>
+        <v>712</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>292</v>
+        <v>26</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>713</v>
+        <v>671</v>
       </c>
     </row>
     <row r="697" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A697" s="1" t="s">
-        <v>291</v>
+        <v>505</v>
       </c>
       <c r="B697" s="1" t="s">
         <v>292</v>
@@ -10452,18 +10455,18 @@
     </row>
     <row r="698" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A698" s="1" t="s">
-        <v>699</v>
+        <v>291</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>48</v>
+        <v>292</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="699" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A699" s="1" t="s">
-        <v>715</v>
+        <v>699</v>
       </c>
       <c r="B699" s="1" t="s">
         <v>48</v>
@@ -10474,7 +10477,7 @@
     </row>
     <row r="700" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A700" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B700" s="1" t="s">
         <v>48</v>
@@ -10485,7 +10488,7 @@
     </row>
     <row r="701" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A701" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B701" s="1" t="s">
         <v>48</v>
@@ -10495,22 +10498,22 @@
       </c>
     </row>
     <row r="702" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A702" s="4" t="s">
-        <v>718</v>
+      <c r="A702" s="1" t="s">
+        <v>717</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>719</v>
+        <v>48</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
     </row>
     <row r="703" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A703" s="4" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B703" s="1" t="s">
-        <v>503</v>
+        <v>719</v>
       </c>
       <c r="C703" s="1" t="s">
         <v>720</v>
@@ -10518,7 +10521,7 @@
     </row>
     <row r="704" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A704" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B704" s="1" t="s">
         <v>503</v>
@@ -10529,7 +10532,7 @@
     </row>
     <row r="705" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A705" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B705" s="1" t="s">
         <v>503</v>
@@ -10540,10 +10543,10 @@
     </row>
     <row r="706" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A706" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>725</v>
+        <v>503</v>
       </c>
       <c r="C706" s="1" t="s">
         <v>720</v>
@@ -10551,7 +10554,7 @@
     </row>
     <row r="707" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A707" s="4" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B707" s="1" t="s">
         <v>725</v>
@@ -10562,10 +10565,10 @@
     </row>
     <row r="708" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A708" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>503</v>
+        <v>725</v>
       </c>
       <c r="C708" s="1" t="s">
         <v>720</v>
@@ -10573,7 +10576,7 @@
     </row>
     <row r="709" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A709" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B709" s="1" t="s">
         <v>503</v>
@@ -10584,10 +10587,10 @@
     </row>
     <row r="710" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A710" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B710" s="1" t="s">
-        <v>725</v>
+        <v>503</v>
       </c>
       <c r="C710" s="1" t="s">
         <v>720</v>
@@ -10595,10 +10598,10 @@
     </row>
     <row r="711" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A711" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>503</v>
+        <v>725</v>
       </c>
       <c r="C711" s="1" t="s">
         <v>720</v>
@@ -10606,7 +10609,7 @@
     </row>
     <row r="712" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A712" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B712" s="1" t="s">
         <v>503</v>
@@ -10617,7 +10620,7 @@
     </row>
     <row r="713" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A713" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B713" s="1" t="s">
         <v>503</v>
@@ -10628,7 +10631,7 @@
     </row>
     <row r="714" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A714" s="4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B714" s="1" t="s">
         <v>503</v>
@@ -10639,7 +10642,7 @@
     </row>
     <row r="715" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A715" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B715" s="1" t="s">
         <v>503</v>
@@ -10650,10 +10653,10 @@
     </row>
     <row r="716" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A716" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B716" s="1" t="s">
-        <v>725</v>
+        <v>503</v>
       </c>
       <c r="C716" s="1" t="s">
         <v>720</v>
@@ -10661,7 +10664,7 @@
     </row>
     <row r="717" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A717" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B717" s="1" t="s">
         <v>725</v>
@@ -10672,10 +10675,10 @@
     </row>
     <row r="718" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A718" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="C718" s="1" t="s">
         <v>720</v>
@@ -10683,10 +10686,10 @@
     </row>
     <row r="719" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A719" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="C719" s="1" t="s">
         <v>720</v>
@@ -10694,7 +10697,7 @@
     </row>
     <row r="720" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A720" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B720" s="1" t="s">
         <v>725</v>
@@ -10705,10 +10708,10 @@
     </row>
     <row r="721" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A721" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>503</v>
+        <v>725</v>
       </c>
       <c r="C721" s="1" t="s">
         <v>720</v>
@@ -10716,10 +10719,10 @@
     </row>
     <row r="722" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A722" s="4" t="s">
-        <v>432</v>
+        <v>740</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>719</v>
+        <v>503</v>
       </c>
       <c r="C722" s="1" t="s">
         <v>720</v>
@@ -10727,10 +10730,10 @@
     </row>
     <row r="723" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A723" s="4" t="s">
-        <v>741</v>
+        <v>432</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>503</v>
+        <v>719</v>
       </c>
       <c r="C723" s="1" t="s">
         <v>720</v>
@@ -10738,10 +10741,10 @@
     </row>
     <row r="724" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A724" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>743</v>
+        <v>503</v>
       </c>
       <c r="C724" s="1" t="s">
         <v>720</v>
@@ -10749,7 +10752,7 @@
     </row>
     <row r="725" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A725" s="4" t="s">
-        <v>291</v>
+        <v>742</v>
       </c>
       <c r="B725" s="1" t="s">
         <v>743</v>
@@ -10763,26 +10766,26 @@
         <v>291</v>
       </c>
       <c r="B726" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C726" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A727" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B727" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C726" s="1" t="s">
+      <c r="C727" s="1" t="s">
         <v>744</v>
-      </c>
-    </row>
-    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A727" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="B727" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="C727" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="728" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A728" s="1" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="B728" s="1" t="s">
         <v>745</v>
@@ -10793,7 +10796,7 @@
     </row>
     <row r="729" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A729" s="1" t="s">
-        <v>24</v>
+        <v>573</v>
       </c>
       <c r="B729" s="1" t="s">
         <v>745</v>
@@ -10804,7 +10807,7 @@
     </row>
     <row r="730" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A730" s="1" t="s">
-        <v>574</v>
+        <v>24</v>
       </c>
       <c r="B730" s="1" t="s">
         <v>745</v>
@@ -10815,7 +10818,7 @@
     </row>
     <row r="731" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A731" s="1" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="B731" s="1" t="s">
         <v>745</v>
@@ -10826,7 +10829,7 @@
     </row>
     <row r="732" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A732" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B732" s="1" t="s">
         <v>745</v>
@@ -10837,7 +10840,7 @@
     </row>
     <row r="733" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A733" s="1" t="s">
-        <v>28</v>
+        <v>598</v>
       </c>
       <c r="B733" s="1" t="s">
         <v>745</v>
@@ -10848,7 +10851,7 @@
     </row>
     <row r="734" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A734" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B734" s="1" t="s">
         <v>745</v>
@@ -10859,7 +10862,7 @@
     </row>
     <row r="735" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A735" s="1" t="s">
-        <v>348</v>
+        <v>35</v>
       </c>
       <c r="B735" s="1" t="s">
         <v>745</v>
@@ -10870,7 +10873,7 @@
     </row>
     <row r="736" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A736" s="1" t="s">
-        <v>600</v>
+        <v>348</v>
       </c>
       <c r="B736" s="1" t="s">
         <v>745</v>
@@ -10881,10 +10884,10 @@
     </row>
     <row r="737" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A737" s="1" t="s">
-        <v>4</v>
+        <v>600</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>523</v>
+        <v>745</v>
       </c>
       <c r="C737" s="1" t="s">
         <v>524</v>
@@ -10892,7 +10895,7 @@
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A738" s="1" t="s">
-        <v>582</v>
+        <v>4</v>
       </c>
       <c r="B738" s="1" t="s">
         <v>523</v>
@@ -10903,7 +10906,7 @@
     </row>
     <row r="739" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A739" s="1" t="s">
-        <v>7</v>
+        <v>582</v>
       </c>
       <c r="B739" s="1" t="s">
         <v>523</v>
@@ -10914,7 +10917,7 @@
     </row>
     <row r="740" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A740" s="1" t="s">
-        <v>576</v>
+        <v>7</v>
       </c>
       <c r="B740" s="1" t="s">
         <v>523</v>
@@ -10925,7 +10928,7 @@
     </row>
     <row r="741" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A741" s="1" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="B741" s="1" t="s">
         <v>523</v>
@@ -10936,7 +10939,7 @@
     </row>
     <row r="742" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A742" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B742" s="1" t="s">
         <v>523</v>
@@ -10947,7 +10950,7 @@
     </row>
     <row r="743" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A743" s="1" t="s">
-        <v>15</v>
+        <v>585</v>
       </c>
       <c r="B743" s="1" t="s">
         <v>523</v>
@@ -10958,7 +10961,7 @@
     </row>
     <row r="744" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A744" s="1" t="s">
-        <v>583</v>
+        <v>15</v>
       </c>
       <c r="B744" s="1" t="s">
         <v>523</v>
@@ -10969,7 +10972,7 @@
     </row>
     <row r="745" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A745" s="1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B745" s="1" t="s">
         <v>523</v>
@@ -10980,7 +10983,7 @@
     </row>
     <row r="746" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A746" s="1" t="s">
-        <v>104</v>
+        <v>586</v>
       </c>
       <c r="B746" s="1" t="s">
         <v>523</v>
@@ -10991,7 +10994,7 @@
     </row>
     <row r="747" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A747" s="1" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="B747" s="1" t="s">
         <v>523</v>
@@ -11002,7 +11005,7 @@
     </row>
     <row r="748" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A748" s="1" t="s">
-        <v>587</v>
+        <v>19</v>
       </c>
       <c r="B748" s="1" t="s">
         <v>523</v>
@@ -11013,7 +11016,7 @@
     </row>
     <row r="749" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A749" s="1" t="s">
-        <v>21</v>
+        <v>587</v>
       </c>
       <c r="B749" s="1" t="s">
         <v>523</v>
@@ -11024,7 +11027,7 @@
     </row>
     <row r="750" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A750" s="1" t="s">
-        <v>577</v>
+        <v>21</v>
       </c>
       <c r="B750" s="1" t="s">
         <v>523</v>
@@ -11035,7 +11038,7 @@
     </row>
     <row r="751" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A751" s="1" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="B751" s="1" t="s">
         <v>523</v>
@@ -11046,7 +11049,7 @@
     </row>
     <row r="752" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A752" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B752" s="1" t="s">
         <v>523</v>
@@ -11057,7 +11060,7 @@
     </row>
     <row r="753" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A753" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B753" s="1" t="s">
         <v>523</v>
@@ -11068,7 +11071,7 @@
     </row>
     <row r="754" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A754" s="1" t="s">
-        <v>366</v>
+        <v>590</v>
       </c>
       <c r="B754" s="1" t="s">
         <v>523</v>
@@ -11079,7 +11082,7 @@
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A755" s="1" t="s">
-        <v>578</v>
+        <v>366</v>
       </c>
       <c r="B755" s="1" t="s">
         <v>523</v>
@@ -11090,7 +11093,7 @@
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A756" s="1" t="s">
-        <v>26</v>
+        <v>578</v>
       </c>
       <c r="B756" s="1" t="s">
         <v>523</v>
@@ -11101,7 +11104,7 @@
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A757" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B757" s="1" t="s">
         <v>523</v>
@@ -11112,7 +11115,7 @@
     </row>
     <row r="758" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A758" s="1" t="s">
-        <v>579</v>
+        <v>48</v>
       </c>
       <c r="B758" s="1" t="s">
         <v>523</v>
@@ -11123,7 +11126,7 @@
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A759" s="1" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
       <c r="B759" s="1" t="s">
         <v>523</v>
@@ -11134,7 +11137,7 @@
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A760" s="1" t="s">
-        <v>580</v>
+        <v>591</v>
       </c>
       <c r="B760" s="1" t="s">
         <v>523</v>
@@ -11145,7 +11148,7 @@
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A761" s="1" t="s">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="B761" s="1" t="s">
         <v>523</v>
@@ -11156,7 +11159,7 @@
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A762" s="1" t="s">
-        <v>592</v>
+        <v>570</v>
       </c>
       <c r="B762" s="1" t="s">
         <v>523</v>
@@ -11167,7 +11170,7 @@
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A763" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B763" s="1" t="s">
         <v>523</v>
@@ -11178,7 +11181,7 @@
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A764" s="1" t="s">
-        <v>571</v>
+        <v>593</v>
       </c>
       <c r="B764" s="1" t="s">
         <v>523</v>
@@ -11189,7 +11192,7 @@
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A765" s="1" t="s">
-        <v>594</v>
+        <v>571</v>
       </c>
       <c r="B765" s="1" t="s">
         <v>523</v>
@@ -11200,7 +11203,7 @@
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A766" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B766" s="1" t="s">
         <v>523</v>
@@ -11211,7 +11214,7 @@
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A767" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B767" s="1" t="s">
         <v>523</v>
@@ -11222,7 +11225,7 @@
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A768" s="1" t="s">
-        <v>581</v>
+        <v>596</v>
       </c>
       <c r="B768" s="1" t="s">
         <v>523</v>
@@ -11233,7 +11236,7 @@
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A769" s="1" t="s">
-        <v>597</v>
+        <v>581</v>
       </c>
       <c r="B769" s="1" t="s">
         <v>523</v>
@@ -11244,10 +11247,10 @@
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A770" s="1" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B770" s="1" t="s">
-        <v>746</v>
+        <v>523</v>
       </c>
       <c r="C770" s="1" t="s">
         <v>524</v>
@@ -11255,10 +11258,10 @@
     </row>
     <row r="771" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A771" s="1" t="s">
-        <v>291</v>
+        <v>601</v>
       </c>
       <c r="B771" s="1" t="s">
-        <v>83</v>
+        <v>746</v>
       </c>
       <c r="C771" s="1" t="s">
         <v>524</v>
@@ -11266,7 +11269,7 @@
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A772" s="1" t="s">
-        <v>394</v>
+        <v>291</v>
       </c>
       <c r="B772" s="1" t="s">
         <v>83</v>
@@ -11276,22 +11279,22 @@
       </c>
     </row>
     <row r="773" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A773" s="4" t="s">
-        <v>747</v>
-      </c>
-      <c r="B773" s="4" t="s">
-        <v>748</v>
+      <c r="A773" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B773" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C773" s="1" t="s">
-        <v>749</v>
+        <v>524</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A774" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="B774" s="1" t="s">
-        <v>722</v>
+        <v>747</v>
+      </c>
+      <c r="B774" s="4" t="s">
+        <v>748</v>
       </c>
       <c r="C774" s="1" t="s">
         <v>749</v>
@@ -11299,7 +11302,7 @@
     </row>
     <row r="775" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A775" s="4" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B775" s="1" t="s">
         <v>722</v>
@@ -11310,7 +11313,7 @@
     </row>
     <row r="776" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A776" s="4" t="s">
-        <v>431</v>
+        <v>751</v>
       </c>
       <c r="B776" s="1" t="s">
         <v>722</v>
@@ -11321,7 +11324,7 @@
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A777" s="4" t="s">
-        <v>752</v>
+        <v>431</v>
       </c>
       <c r="B777" s="1" t="s">
         <v>722</v>
@@ -11332,21 +11335,21 @@
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A778" s="4" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>748</v>
+        <v>722</v>
       </c>
       <c r="C778" s="1" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="779" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A779" s="1" t="s">
-        <v>291</v>
+      <c r="A779" s="4" t="s">
+        <v>753</v>
       </c>
       <c r="B779" s="1" t="s">
-        <v>83</v>
+        <v>748</v>
       </c>
       <c r="C779" s="1" t="s">
         <v>749</v>
@@ -11357,15 +11360,15 @@
         <v>291</v>
       </c>
       <c r="B780" s="1" t="s">
-        <v>292</v>
+        <v>83</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A781" s="1" t="s">
-        <v>371</v>
+        <v>291</v>
       </c>
       <c r="B781" s="1" t="s">
         <v>292</v>
@@ -11376,21 +11379,21 @@
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A782" s="1" t="s">
-        <v>427</v>
+        <v>371</v>
       </c>
       <c r="B782" s="1" t="s">
-        <v>425</v>
+        <v>292</v>
       </c>
       <c r="C782" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="783" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A783" s="1" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B783" s="1" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C783" s="1" t="s">
         <v>755</v>
@@ -11398,10 +11401,10 @@
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A784" s="1" t="s">
-        <v>291</v>
+        <v>424</v>
       </c>
       <c r="B784" s="1" t="s">
-        <v>83</v>
+        <v>422</v>
       </c>
       <c r="C784" s="1" t="s">
         <v>755</v>
@@ -11409,18 +11412,18 @@
     </row>
     <row r="785" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A785" s="1" t="s">
-        <v>427</v>
+        <v>291</v>
       </c>
       <c r="B785" s="1" t="s">
-        <v>756</v>
+        <v>83</v>
       </c>
       <c r="C785" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A786" s="1" t="s">
-        <v>758</v>
+        <v>427</v>
       </c>
       <c r="B786" s="1" t="s">
         <v>756</v>
@@ -11431,7 +11434,7 @@
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A787" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B787" s="1" t="s">
         <v>756</v>
@@ -11442,10 +11445,10 @@
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A788" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B788" s="1" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="C788" s="1" t="s">
         <v>757</v>
@@ -11453,7 +11456,7 @@
     </row>
     <row r="789" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A789" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B789" s="1" t="s">
         <v>761</v>
@@ -11464,7 +11467,7 @@
     </row>
     <row r="790" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A790" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B790" s="1" t="s">
         <v>761</v>
@@ -11475,10 +11478,10 @@
     </row>
     <row r="791" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A791" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C791" s="1" t="s">
         <v>757</v>
@@ -11486,7 +11489,7 @@
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A792" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B792" s="1" t="s">
         <v>765</v>
@@ -11497,10 +11500,10 @@
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A793" s="1" t="s">
-        <v>394</v>
+        <v>766</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>83</v>
+        <v>765</v>
       </c>
       <c r="C793" s="1" t="s">
         <v>757</v>
@@ -11508,7 +11511,7 @@
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A794" s="1" t="s">
-        <v>291</v>
+        <v>394</v>
       </c>
       <c r="B794" s="1" t="s">
         <v>83</v>
@@ -11517,8 +11520,19 @@
         <v>757</v>
       </c>
     </row>
+    <row r="795" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A795" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B795" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C795" s="1" t="s">
+        <v>757</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C701" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C702" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>

</xml_diff>